<commit_message>
added java doc : Manish
</commit_message>
<xml_diff>
--- a/src/test/resources/testdataSheet/testdata.xlsx
+++ b/src/test/resources/testdataSheet/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\FarmSoilAutomation\src\test\resources\testdataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9953B3F-2267-4D07-B56E-2FEAB5F97442}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20CF886-D703-4512-8B0D-E179FA200CD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>terminalID</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>CURRENCYDISPENSER1</t>
+  </si>
+  <si>
+    <t>TimeStamp</t>
+  </si>
+  <si>
+    <t>11/26/2020 2:42:15 AM</t>
   </si>
 </sst>
 </file>
@@ -366,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -411,6 +417,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated excel sheet : Manish
</commit_message>
<xml_diff>
--- a/src/test/resources/testdataSheet/testdata.xlsx
+++ b/src/test/resources/testdataSheet/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\FarmSoilAutomation\src\test\resources\testdataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20CF886-D703-4512-8B0D-E179FA200CD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CA662B-DC7D-4991-842F-4495C748CE37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>terminalID</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>11/26/2020 2:42:15 AM</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -375,7 +378,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -411,7 +414,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
added script to read from excel sheet : Manish
</commit_message>
<xml_diff>
--- a/src/test/resources/testdataSheet/testdata.xlsx
+++ b/src/test/resources/testdataSheet/testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\FarmSoilAutomation\src\test\resources\testdataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CA662B-DC7D-4991-842F-4495C748CE37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D092F04-707E-404D-A384-CEADFFC064AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="24">
   <si>
     <t>terminalID</t>
   </si>
@@ -58,19 +59,64 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Terminal_ID</t>
+  </si>
+  <si>
+    <t>Device vendor identity</t>
+  </si>
+  <si>
+    <t>Motorized Card Reader</t>
+  </si>
+  <si>
+    <t>Capture Bin 1</t>
+  </si>
+  <si>
+    <t>RETAIN BIN OK                                                                                       </t>
+  </si>
+  <si>
+    <t>Instance_id</t>
+  </si>
+  <si>
+    <t>deviceId</t>
+  </si>
+  <si>
+    <t>Device_Status</t>
+  </si>
+  <si>
+    <t>Device_description</t>
+  </si>
+  <si>
+    <t>Sub_device_name</t>
+  </si>
+  <si>
+    <t>Sub_device_status</t>
+  </si>
+  <si>
+    <t>Sub_device_description</t>
+  </si>
+  <si>
+    <t>CARD READER ONLINE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,8 +139,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,17 +426,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -398,7 +447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -409,7 +458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -420,7 +469,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -435,4 +484,172 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DEBFAE3-EA56-4175-A635-D279F18F8960}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="52.28515625" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added some test : Manish
</commit_message>
<xml_diff>
--- a/src/test/resources/testdataSheet/testdata.xlsx
+++ b/src/test/resources/testdataSheet/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\FarmSoilAutomation\src\test\resources\testdataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D092F04-707E-404D-A384-CEADFFC064AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4700CC-CA0F-40E4-B527-DDCF59505CF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
   <si>
     <t>terminalID</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>CARD READER ONLINE</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -139,9 +145,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -427,16 +436,16 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,7 +456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -458,7 +467,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -469,7 +478,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -491,20 +500,20 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="52.28515625" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" customWidth="1"/>
+    <col min="5" max="5" width="52.26953125" customWidth="1"/>
+    <col min="7" max="7" width="26.1796875" customWidth="1"/>
+    <col min="8" max="8" width="17.7265625" customWidth="1"/>
+    <col min="9" max="9" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="33" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -533,12 +542,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="33" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>1</v>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -562,12 +571,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="82.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="82.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
-        <v>2</v>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
@@ -591,7 +600,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="33" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -620,7 +629,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="82.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="82.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
fixed code : Manish
</commit_message>
<xml_diff>
--- a/src/test/resources/testdataSheet/testdata.xlsx
+++ b/src/test/resources/testdataSheet/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\FarmSoilAutomation\src\test\resources\testdataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4700CC-CA0F-40E4-B527-DDCF59505CF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39DF0B7-57A9-484F-BADE-7FF7218BF630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
   <si>
     <t>terminalID</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Capture Bin 1</t>
   </si>
   <si>
-    <t>RETAIN BIN OK                                                                                       </t>
-  </si>
-  <si>
     <t>Instance_id</t>
   </si>
   <si>
@@ -104,6 +101,9 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>RETAIN BIN OK</t>
   </si>
 </sst>
 </file>
@@ -439,13 +439,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,7 +456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -467,7 +467,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -478,7 +478,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -499,55 +499,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DEBFAE3-EA56-4175-A635-D279F18F8960}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.1796875" customWidth="1"/>
-    <col min="3" max="3" width="18.81640625" customWidth="1"/>
-    <col min="5" max="5" width="52.26953125" customWidth="1"/>
-    <col min="7" max="7" width="26.1796875" customWidth="1"/>
-    <col min="8" max="8" width="17.7265625" customWidth="1"/>
-    <col min="9" max="9" width="16.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="33" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="33" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -556,7 +554,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
@@ -571,12 +569,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="82.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="33" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
@@ -588,24 +586,24 @@
         <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="33" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="33" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
-        <v>1</v>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
@@ -614,7 +612,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>10</v>
@@ -629,12 +627,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="82.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="33" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
-        <v>1</v>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -652,7 +650,7 @@
         <v>10</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
added some more code : Manish
</commit_message>
<xml_diff>
--- a/src/test/resources/testdataSheet/testdata.xlsx
+++ b/src/test/resources/testdataSheet/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\FarmSoilAutomation\src\test\resources\testdataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39DF0B7-57A9-484F-BADE-7FF7218BF630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681A7922-E6AA-475E-A948-6B65FEC0F188}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -435,17 +435,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,7 +457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -467,7 +468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -478,7 +479,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -499,19 +500,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DEBFAE3-EA56-4175-A635-D279F18F8960}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" customWidth="1"/>
+    <col min="5" max="5" width="24.26953125" customWidth="1"/>
+    <col min="7" max="7" width="26.1796875" customWidth="1"/>
+    <col min="8" max="8" width="17.7265625" customWidth="1"/>
+    <col min="9" max="9" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="33" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -540,7 +541,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="33" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -569,7 +570,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="33" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -598,7 +599,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="33" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -627,7 +628,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="33" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
added some more codes : Manish
</commit_message>
<xml_diff>
--- a/src/test/resources/testdataSheet/testdata.xlsx
+++ b/src/test/resources/testdataSheet/testdata.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\FarmSoilAutomation\src\test\resources\testdataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681A7922-E6AA-475E-A948-6B65FEC0F188}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590B359E-9736-4B92-A714-49E8BBE7B6D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="47">
   <si>
     <t>terminalID</t>
   </si>
@@ -104,6 +105,69 @@
   </si>
   <si>
     <t>RETAIN BIN OK</t>
+  </si>
+  <si>
+    <t>manish</t>
+  </si>
+  <si>
+    <t>ashish</t>
+  </si>
+  <si>
+    <t>IDC01S1</t>
+  </si>
+  <si>
+    <t>IDC01S2</t>
+  </si>
+  <si>
+    <t>statusCode</t>
+  </si>
+  <si>
+    <t>deviceState</t>
+  </si>
+  <si>
+    <t>deviceInstance</t>
+  </si>
+  <si>
+    <t>deviceName</t>
+  </si>
+  <si>
+    <t>deviceDescription</t>
+  </si>
+  <si>
+    <t>deviceVendorIdentity</t>
+  </si>
+  <si>
+    <t>subDeviceName</t>
+  </si>
+  <si>
+    <t>subDeviceState</t>
+  </si>
+  <si>
+    <t>subDeviceDescription</t>
+  </si>
+  <si>
+    <t>IDC01S3</t>
+  </si>
+  <si>
+    <t>IDC01S4</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Recycler1</t>
+  </si>
+  <si>
+    <t>Recycler2</t>
+  </si>
+  <si>
+    <t>Recycler3</t>
+  </si>
+  <si>
+    <t>Recycler4</t>
   </si>
 </sst>
 </file>
@@ -145,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -153,6 +217,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,18 +500,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.26953125" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,7 +522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -468,7 +533,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -479,7 +544,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -500,19 +565,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DEBFAE3-EA56-4175-A635-D279F18F8960}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.1796875" customWidth="1"/>
-    <col min="3" max="3" width="18.81640625" customWidth="1"/>
-    <col min="5" max="5" width="24.26953125" customWidth="1"/>
-    <col min="7" max="7" width="26.1796875" customWidth="1"/>
-    <col min="8" max="8" width="17.7265625" customWidth="1"/>
-    <col min="9" max="9" width="16.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -541,7 +608,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="33" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -549,7 +616,7 @@
         <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>10</v>
@@ -570,7 +637,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -578,7 +645,7 @@
         <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
@@ -599,7 +666,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="33" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="33" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -628,7 +695,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="33" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="33" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -654,6 +721,176 @@
         <v>25</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816B1B8C-9B74-4F32-B266-40E57AC2A1C8}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>